<commit_message>
Add automation code for Hackathon GenAI-testcase-generator
</commit_message>
<xml_diff>
--- a/static/temp/user_story_test_cases.xlsx
+++ b/static/temp/user_story_test_cases.xlsx
@@ -27,57 +27,58 @@
   <si>
     <t>**Positive Test Cases:**
 **Test Case ID:** 001
-**Description:** Verify employee can successfully authenticate using OTP sent to official email.
-**Preconditions:** Employee has a valid official email registered in the system.
-**Steps:**
-1. Employee enters their email address on the OTP authentication page.
-2. Employee receives OTP on their official email.
-3. Employee enters the OTP on the authentication page.
-**Expected Results:** Employee successfully logs in and can access HR-related information via WhatsApp.
+**Description:** User successfully authenticates using OTP sent to official email.
+**Preconditions:** User has access to their official email.
+**Steps:**
+1. User enters their email address on the HR portal.
+2. User requests OTP.
+3. User checks their official email and retrieves the OTP.
+4. User enters the OTP on the HR portal.
+**Expected Results:** User is successfully authenticated and can access HR-related information via WhatsApp.
 **Priority:** High
 **Validation Test Cases:**
 **Test Case ID:** 002
-**Description:** Verify error message is displayed if employee enters incorrect OTP.
-**Preconditions:** Employee has received an OTP on their official email.
-**Steps:**
-1. Employee enters the incorrect OTP on the authentication page.
-**Expected Results:** Error message is displayed indicating incorrect OTP.
+**Description:** User enters an incorrect email address.
+**Preconditions:** User has access to the HR portal.
+**Steps:**
+1. User enters an incorrect email address on the HR portal.
+2. User requests OTP.
+**Expected Results:** System displays an error message prompting the user to enter a valid email address.
 **Priority:** Medium
 **UI/UX Test Cases:**
 **Test Case ID:** 003
-**Description:** Verify OTP authentication page has a user-friendly design.
-**Preconditions:** Employee is on the OTP authentication page.
-**Steps:**
-1. Check the layout and design of the OTP authentication page.
-**Expected Results:** OTP authentication page is intuitive and easy to use.
+**Description:** OTP request button is clearly visible and accessible on the HR portal.
+**Preconditions:** User has access to the HR portal.
+**Steps:**
+1. User navigates to the authentication page on the HR portal.
+**Expected Results:** OTP request button is prominent and easy to locate on the page.
 **Priority:** Medium
 **Performance Test Cases:**
 **Test Case ID:** 004
-**Description:** Verify OTP is received promptly on the official email.
-**Preconditions:** Employee is on the OTP authentication page.
-**Steps:**
-1. Employee requests OTP.
-2. Measure the time taken for the OTP to be received on the official email.
-**Expected Results:** OTP is received within a reasonable timeframe.
+**Description:** Test system performance when multiple users are simultaneously requesting OTPs.
+**Preconditions:** Multiple users are accessing the HR portal.
+**Steps:**
+1. Multiple users request OTPs simultaneously.
+**Expected Results:** System should be able to handle the load and deliver OTPs promptly to all users.
 **Priority:** High
 **Security Test Cases:**
 **Test Case ID:** 005
-**Description:** Verify OTP is valid only for a single use.
-**Preconditions:** Employee has received an OTP on the official email.
-**Steps:**
-1. Employee uses the OTP to log in successfully.
-2. Employee tries to use the same OTP again.
-**Expected Results:** OTP is no longer valid for reuse.
+**Description:** Test if OTPs are valid only for a limited time.
+**Preconditions:** User receives OTP.
+**Steps:**
+1. User retrieves OTP and waits for a significant amount of time.
+2. User tries to enter the same OTP after the validity period has passed.
+**Expected Results:** System should not accept the expired OTP and prompt the user to request a new one.
 **Priority:** High
 **Combination Test Cases:**
 **Test Case ID:** 006
-**Description:** Verify employee can authenticate using OTP on different devices.
-**Preconditions:** Employee has access to multiple devices.
-**Steps:**
-1. Employee logs in on one device using the OTP.
-2. Employee tries to log in on another device using the same OTP.
-**Expected Results:** Employee can successfully log in on both devices using the same OTP.
-**Priority:** High</t>
+**Description:** User enters an incorrect email address and then requests OTP.
+**Preconditions:** User has access to the HR portal.
+**Steps:**
+1. User enters an incorrect email address on the HR portal.
+2. User requests OTP.
+**Expected Results:** System should display an error message for the incorrect email address and not send an OTP.
+**Priority:** Medium</t>
   </si>
 </sst>
 </file>

</xml_diff>